<commit_message>
Sheet for each cable type
</commit_message>
<xml_diff>
--- a/Cables.xlsx
+++ b/Cables.xlsx
@@ -5,15 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Dwen\Dropbox\SouthSeas Upgrade 2015\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ssftvstudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14550" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14550"/>
   </bookViews>
   <sheets>
-    <sheet name="1XXX Ref" sheetId="1" r:id="rId1"/>
-    <sheet name="2XXX HD-SDI" sheetId="2" r:id="rId2"/>
+    <sheet name="1XXX HD-SDI" sheetId="1" r:id="rId1"/>
+    <sheet name="2XXX Ref" sheetId="2" r:id="rId2"/>
+    <sheet name="3XXX Network" sheetId="3" r:id="rId3"/>
+    <sheet name="4XXX Audio" sheetId="4" r:id="rId4"/>
+    <sheet name="5XXX Coms" sheetId="5" r:id="rId5"/>
+    <sheet name="6XXX Timcode" sheetId="6" r:id="rId6"/>
+    <sheet name="7XXX KVM" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="7">
   <si>
     <t>Cable#</t>
   </si>
@@ -433,11 +438,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -671,66 +676,6 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="1">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="1">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="1">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" s="1">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" s="1">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="1">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" s="1">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" s="1">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="1">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" s="1">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="1">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" s="1">
-        <v>1050</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -739,11 +684,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -977,64 +922,1234 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="1">
-        <v>2039</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="1">
-        <v>2040</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="1">
-        <v>2041</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" s="1">
-        <v>2042</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" s="1">
-        <v>2043</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="1">
-        <v>2044</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" s="1">
-        <v>2045</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" s="1">
-        <v>2046</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="1">
-        <v>2047</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" s="1">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="1">
-        <v>2049</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" s="1">
-        <v>2050</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="4" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" customWidth="1"/>
+    <col min="7" max="8" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>3023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>3031</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>3032</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>3033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>3034</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>3035</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>3037</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>3038</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="4" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" customWidth="1"/>
+    <col min="7" max="8" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>4001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>4002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>4003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>4004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>4005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>4006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>4007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>4008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>4010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>4011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>4012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>4014</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>4015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>4016</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>4017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>4018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>4019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>4021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>4022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>4023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>4024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>4025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>4026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>4027</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>4028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>4029</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>4030</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>4031</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>4032</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>4033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>4034</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>4035</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>4036</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>4037</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>4038</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="4" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" customWidth="1"/>
+    <col min="7" max="8" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>5001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>5002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>5003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>5005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>5006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>5007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>5008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>5009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>5010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>5011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>5012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>5013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>5014</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>5015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>5016</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>5017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>5018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>5019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>5020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>5021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>5022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>5023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>5024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>5025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>5026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>5027</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>5028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>5029</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>5030</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>5031</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>5032</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>5033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>5034</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>5035</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>5036</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>5037</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>5038</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="4" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" customWidth="1"/>
+    <col min="7" max="8" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>6001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>6002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>6003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>6004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>6006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>6007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>6008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>6009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>6010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>6011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>6012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>6013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>6014</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>6015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>6016</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>6017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>6018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>6019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>6020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>6021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>6022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>6023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>6024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>6025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>6026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>6027</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>6028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>6029</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>6030</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>6031</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>6032</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>6033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>6034</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>6035</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>6036</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>6037</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>6038</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="4" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" customWidth="1"/>
+    <col min="7" max="8" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>7001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>7002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>7003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>7004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>7005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>7007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>7008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>7009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>7010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>7011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>7012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>7013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>7014</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>7015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>7016</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>7017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>7018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>7019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>7020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>7021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>7022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>7023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>7024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>7025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>7026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>7027</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>7028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>7029</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>7030</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>7031</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>7032</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>7033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>7034</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>7035</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>7036</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>7037</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>7038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove RTR Panel 02
ACR will use software panels
</commit_message>
<xml_diff>
--- a/Cables.xlsx
+++ b/Cables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14550" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14550" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1-Ref" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="363">
   <si>
     <t>Cable#</t>
   </si>
@@ -916,9 +916,6 @@
     <t>Audio Mixer 01</t>
   </si>
   <si>
-    <t>RTR Panel 02</t>
-  </si>
-  <si>
     <t>DVI O/P</t>
   </si>
   <si>
@@ -1121,6 +1118,9 @@
   </si>
   <si>
     <t>E14</t>
+  </si>
+  <si>
+    <t>I/O 43</t>
   </si>
 </sst>
 </file>
@@ -1794,7 +1794,7 @@
         <v>156</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>8</v>
@@ -1865,7 +1865,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -1891,7 +1891,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -1917,7 +1917,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -1943,7 +1943,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -1969,7 +1969,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -1986,7 +1986,7 @@
         <v>2006</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
@@ -2003,7 +2003,7 @@
         <v>2007</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -2020,7 +2020,7 @@
         <v>2008</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
@@ -2757,7 +2757,7 @@
         <v>156</v>
       </c>
       <c r="G45" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H45" t="s">
         <v>8</v>
@@ -2807,7 +2807,7 @@
         <v>8</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F52" t="s">
         <v>33</v>
@@ -2833,7 +2833,7 @@
         <v>8</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F53" t="s">
         <v>35</v>
@@ -2859,7 +2859,7 @@
         <v>8</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F54" t="s">
         <v>36</v>
@@ -2885,7 +2885,7 @@
         <v>8</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F55" t="s">
         <v>37</v>
@@ -2911,7 +2911,7 @@
         <v>8</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F56" t="s">
         <v>38</v>
@@ -2941,7 +2941,7 @@
         <v>156</v>
       </c>
       <c r="G57" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H57" t="s">
         <v>8</v>
@@ -2965,7 +2965,7 @@
         <v>156</v>
       </c>
       <c r="G58" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H58" t="s">
         <v>8</v>
@@ -4226,7 +4226,7 @@
         <v>156</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>8</v>
@@ -4249,7 +4249,7 @@
         <v>156</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>8</v>
@@ -4272,7 +4272,7 @@
         <v>156</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>8</v>
@@ -4337,7 +4337,7 @@
         <v>156</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D2" t="s">
         <v>157</v>
@@ -4363,7 +4363,7 @@
         <v>156</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D3" t="s">
         <v>157</v>
@@ -4389,7 +4389,7 @@
         <v>156</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D4" t="s">
         <v>157</v>
@@ -4415,7 +4415,7 @@
         <v>156</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D5" t="s">
         <v>157</v>
@@ -4441,7 +4441,7 @@
         <v>156</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D6" t="s">
         <v>157</v>
@@ -4467,7 +4467,7 @@
         <v>156</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D7" t="s">
         <v>157</v>
@@ -4493,7 +4493,7 @@
         <v>156</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D8" t="s">
         <v>157</v>
@@ -4519,7 +4519,7 @@
         <v>156</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D9" t="s">
         <v>157</v>
@@ -4545,7 +4545,7 @@
         <v>156</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D10" t="s">
         <v>157</v>
@@ -4571,7 +4571,7 @@
         <v>156</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D11" t="s">
         <v>157</v>
@@ -4597,7 +4597,7 @@
         <v>156</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D12" t="s">
         <v>157</v>
@@ -4623,7 +4623,7 @@
         <v>156</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D13" t="s">
         <v>157</v>
@@ -4649,7 +4649,7 @@
         <v>156</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D14" t="s">
         <v>157</v>
@@ -4675,7 +4675,7 @@
         <v>156</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D15" t="s">
         <v>157</v>
@@ -4701,7 +4701,7 @@
         <v>156</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D16" t="s">
         <v>157</v>
@@ -4727,7 +4727,7 @@
         <v>156</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D17" t="s">
         <v>157</v>
@@ -4753,7 +4753,7 @@
         <v>156</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D18" t="s">
         <v>157</v>
@@ -4779,7 +4779,7 @@
         <v>156</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D19" t="s">
         <v>157</v>
@@ -4805,7 +4805,7 @@
         <v>156</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D20" t="s">
         <v>157</v>
@@ -4831,7 +4831,7 @@
         <v>156</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D21" t="s">
         <v>157</v>
@@ -4857,7 +4857,7 @@
         <v>156</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D22" t="s">
         <v>157</v>
@@ -4883,7 +4883,7 @@
         <v>156</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D23" t="s">
         <v>157</v>
@@ -4909,7 +4909,7 @@
         <v>156</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D24" t="s">
         <v>157</v>
@@ -4935,7 +4935,7 @@
         <v>156</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D25" t="s">
         <v>157</v>
@@ -5527,7 +5527,7 @@
         <v>156</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H54" t="s">
         <v>223</v>
@@ -5553,7 +5553,7 @@
         <v>156</v>
       </c>
       <c r="G55" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H55" t="s">
         <v>223</v>
@@ -5809,7 +5809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
@@ -5867,7 +5867,7 @@
         <v>156</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>29</v>
@@ -5890,7 +5890,7 @@
         <v>156</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>29</v>
@@ -5990,7 +5990,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B8" t="s">
         <v>236</v>
@@ -6013,7 +6013,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B9" t="s">
         <v>236</v>
@@ -6028,7 +6028,7 @@
         <v>156</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>29</v>
@@ -6036,7 +6036,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B10" t="s">
         <v>236</v>
@@ -6051,7 +6051,7 @@
         <v>156</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>29</v>
@@ -6457,9 +6457,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6935,8 +6935,8 @@
       <c r="F25" t="s">
         <v>290</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>29</v>
+      <c r="G25" s="12" t="s">
+        <v>362</v>
       </c>
       <c r="H25" t="s">
         <v>263</v>
@@ -7070,6 +7070,15 @@
       <c r="D32" t="s">
         <v>263</v>
       </c>
+      <c r="F32" t="s">
+        <v>292</v>
+      </c>
+      <c r="G32" t="s">
+        <v>288</v>
+      </c>
+      <c r="H32" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
@@ -7213,15 +7222,6 @@
       <c r="D40" t="s">
         <v>263</v>
       </c>
-      <c r="F40" t="s">
-        <v>292</v>
-      </c>
-      <c r="G40" t="s">
-        <v>288</v>
-      </c>
-      <c r="H40" t="s">
-        <v>263</v>
-      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
@@ -7340,15 +7340,6 @@
         <v>268</v>
       </c>
       <c r="D47" t="s">
-        <v>263</v>
-      </c>
-      <c r="F47" t="s">
-        <v>294</v>
-      </c>
-      <c r="G47" t="s">
-        <v>288</v>
-      </c>
-      <c r="H47" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7439,19 +7430,19 @@
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G2" t="s">
         <v>300</v>
       </c>
-      <c r="G2" t="s">
-        <v>301</v>
-      </c>
       <c r="H2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -7462,19 +7453,19 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -7485,19 +7476,19 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -7508,19 +7499,19 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="25" spans="7:7" x14ac:dyDescent="0.35">
@@ -7588,16 +7579,16 @@
         <v>51</v>
       </c>
       <c r="D2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F2" t="s">
         <v>307</v>
-      </c>
-      <c r="F2" t="s">
-        <v>308</v>
       </c>
       <c r="G2" t="s">
         <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -7605,22 +7596,22 @@
         <v>9002</v>
       </c>
       <c r="B3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G3" t="s">
         <v>96</v>
       </c>
       <c r="H3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" spans="7:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add VMX PC to Network
</commit_message>
<xml_diff>
--- a/Cables.xlsx
+++ b/Cables.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="364">
   <si>
     <t>Cable#</t>
   </si>
@@ -1121,6 +1121,9 @@
   </si>
   <si>
     <t>I/O 43</t>
+  </si>
+  <si>
+    <t>VMX PC</t>
   </si>
 </sst>
 </file>
@@ -6458,8 +6461,8 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7091,6 +7094,15 @@
         <v>270</v>
       </c>
       <c r="D33" t="s">
+        <v>263</v>
+      </c>
+      <c r="F33" t="s">
+        <v>363</v>
+      </c>
+      <c r="G33" t="s">
+        <v>288</v>
+      </c>
+      <c r="H33" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 4K DA for Camera Ret
The VMX control of camera is only on the 4K output.
</commit_message>
<xml_diff>
--- a/Cables.xlsx
+++ b/Cables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14550" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14550" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1-Ref" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="365">
   <si>
     <t>Cable#</t>
   </si>
@@ -1124,6 +1124,9 @@
   </si>
   <si>
     <t>VMX PC</t>
+  </si>
+  <si>
+    <t>A11</t>
   </si>
 </sst>
 </file>
@@ -1813,9 +1816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2425,10 +2428,10 @@
         <v>2030</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
@@ -2704,7 +2707,7 @@
         <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
@@ -2727,7 +2730,7 @@
         <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D44" t="s">
         <v>8</v>
@@ -2940,15 +2943,6 @@
         <v>8</v>
       </c>
       <c r="E57" s="8"/>
-      <c r="F57" t="s">
-        <v>156</v>
-      </c>
-      <c r="G57" t="s">
-        <v>324</v>
-      </c>
-      <c r="H57" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
@@ -2964,15 +2958,6 @@
         <v>8</v>
       </c>
       <c r="E58" s="8"/>
-      <c r="F58" t="s">
-        <v>156</v>
-      </c>
-      <c r="G58" t="s">
-        <v>325</v>
-      </c>
-      <c r="H58" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
@@ -3006,98 +2991,224 @@
       <c r="A61" s="1">
         <v>2060</v>
       </c>
+      <c r="B61" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" t="s">
+        <v>45</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" t="s">
+        <v>30</v>
+      </c>
+      <c r="G61" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>2061</v>
       </c>
+      <c r="B62" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" t="s">
+        <v>45</v>
+      </c>
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>2062</v>
       </c>
+      <c r="B63" t="s">
+        <v>30</v>
+      </c>
+      <c r="C63" t="s">
+        <v>48</v>
+      </c>
+      <c r="D63" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" t="s">
+        <v>156</v>
+      </c>
+      <c r="G63" t="s">
+        <v>324</v>
+      </c>
+      <c r="H63" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>2063</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64" t="s">
+        <v>59</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" t="s">
+        <v>156</v>
+      </c>
+      <c r="G64" t="s">
+        <v>325</v>
+      </c>
+      <c r="H64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>2064</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65" t="s">
+        <v>60</v>
+      </c>
+      <c r="D65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" t="s">
+        <v>156</v>
+      </c>
+      <c r="G65" t="s">
+        <v>364</v>
+      </c>
+      <c r="H65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>2065</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>30</v>
+      </c>
+      <c r="C66" t="s">
+        <v>61</v>
+      </c>
+      <c r="D66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>2066</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" t="s">
+        <v>62</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>2067</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>30</v>
+      </c>
+      <c r="C68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>2068</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>30</v>
+      </c>
+      <c r="C69" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>2069</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70" t="s">
+        <v>65</v>
+      </c>
+      <c r="D70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>2070</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>2071</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>2072</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>2073</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>2074</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>2075</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>2076</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>2077</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>2078</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>2079</v>
       </c>
@@ -6460,9 +6571,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Remove Frame 01 from network
</commit_message>
<xml_diff>
--- a/Cables.xlsx
+++ b/Cables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14550" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14550" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1-Ref" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="369">
   <si>
     <t>Cable#</t>
   </si>
@@ -6216,7 +6216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
@@ -6396,9 +6396,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6517,15 +6517,6 @@
         <v>265</v>
       </c>
       <c r="D5" t="s">
-        <v>261</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>286</v>
-      </c>
-      <c r="H5" t="s">
         <v>261</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Burn RTR outputs for the previous commit
Rather than loop back.
</commit_message>
<xml_diff>
--- a/Cables.xlsx
+++ b/Cables.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="390">
   <si>
     <t>Cable#</t>
   </si>
@@ -1196,9 +1196,6 @@
   </si>
   <si>
     <t>SDI-HDMI 01</t>
-  </si>
-  <si>
-    <t>SDI Loop</t>
   </si>
   <si>
     <t>SDI-HDMI 02</t>
@@ -1956,8 +1953,8 @@
   <dimension ref="A1:H141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2654,51 +2651,51 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="16">
+    <row r="34" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="8">
         <v>2033</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="7" t="s">
+      <c r="B34" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="H34" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="16">
+      <c r="H34" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="8">
         <v>2034</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="7" t="s">
+      <c r="B35" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="H35" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2946,49 +2943,13 @@
       <c r="A46" s="16">
         <v>2045</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="E46" s="17"/>
-      <c r="F46" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="47" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16">
         <v>2046</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>390</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="E47" s="17"/>
-      <c r="F47" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
@@ -4461,51 +4422,51 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="8">
+    <row r="140" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A140" s="16">
         <v>2139</v>
       </c>
-      <c r="B140" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C140" s="9" t="s">
+      <c r="B140" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C140" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D140" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E140" s="10"/>
-      <c r="F140" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G140" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="H140" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="8">
+      <c r="D140" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E140" s="17"/>
+      <c r="F140" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="G140" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H140" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="16">
         <v>2140</v>
       </c>
-      <c r="B141" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C141" s="9" t="s">
+      <c r="B141" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C141" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D141" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E141" s="10"/>
-      <c r="F141" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G141" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="H141" s="9" t="s">
+      <c r="D141" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E141" s="17"/>
+      <c r="F141" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="G141" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H141" s="7" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>